<commit_message>
Updated ICDC MGT01 and OSA03 queries
</commit_message>
<xml_diff>
--- a/InputFiles/ICDC/TC01_ICDC_OSA03_Breed-Boxer.xlsx
+++ b/InputFiles/ICDC/TC01_ICDC_OSA03_Breed-Boxer.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sohilz2/Automation/poc-07-15-2024/Commons_Automation/InputFiles/ICDC/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7D306B5-859C-8C4F-B583-B6F371E5F3E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8307DECA-CBA9-F145-AEB8-2A19A6C4AD8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-45620" yWindow="-4940" windowWidth="42480" windowHeight="27840" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
   </bookViews>
@@ -64,6 +64,48 @@
   </si>
   <si>
     <t>TC01_ICDC_OSA03_Breed-Boxer_TSVData.xlsx</t>
+  </si>
+  <si>
+    <t>SELECT DISTINCT
+    smp.sample_id AS "Sample ID",
+    c.case_record_id AS "Case ID",
+    COALESCE(dmg.breed, '') AS "Breed",
+    COALESCE(diag.disease_term, '') AS "Diagnosis",
+    COALESCE(smp.sample_site, '') AS "Sample Site",
+    COALESCE(smp.summarized_sample_type, '') AS "Sample Type",
+    COALESCE(smp.specific_sample_pathology, '') AS "Pathology/Morphology",
+    COALESCE(smp.tumor_grade, '') AS "Tumor Grade",
+    COALESCE(smp.sample_chronology, '') AS "Sample Chronology",
+    COALESCE(smp.percentage_tumor, '') AS "Percentage Tumor",
+    COALESCE(smp.necropsy_sample, '') AS "Necropsy Sample",
+    COALESCE(smp.sample_preservation, '') AS "Sample Preservation"
+FROM 
+    df_sample smp
+JOIN 
+    df_case c ON smp."case.case_record_id" = c.case_record_id
+JOIN 
+    df_publication pub ON pub."study.clinical_study_designation" = st.clinical_study_designation
+JOIN 
+    df_demographic dmg ON dmg."case.case_record_id" = c.case_record_id
+JOIN 
+    df_diagnosis diag ON diag."case.case_record_id" = c.case_record_id
+JOIN 
+    df_enrollment enr ON enr."case.case_record_id" = c.case_record_id
+JOIN 
+    df_program p ON st."program.program_acronym" = p.program_acronym
+JOIN 
+    df_study st ON c."study.clinical_study_designation" = st.clinical_study_designation
+LEFT JOIN 
+    df_registration reg ON reg."case.case_record_id" = c.case_record_id
+LEFT JOIN 
+    df_case_file cf ON cf."sample.sample_id" = smp.sample_id
+LEFT JOIN 
+    df_study_file sf ON sf."study.clinical_study_designation" = st.clinical_study_designation
+WHERE 
+   st.clinical_study_designation = 'OSA03' AND dmg.breed = 'Boxer'
+ORDER BY 
+    smp.sample_id ASC
+LIMIT 100;</t>
   </si>
   <si>
     <t>SELECT 
@@ -135,102 +177,13 @@
 JOIN 
     df_publication pub ON pub."study.clinical_study_designation" = st.clinical_study_designation
 LEFT JOIN 
+    df_registration reg ON reg."case.case_record_id" = c.case_record_id
+LEFT JOIN 
     df_study_file sf ON sf."study.clinical_study_designation" = st.clinical_study_designation
 WHERE
     st.clinical_study_designation = 'OSA03' AND dmg.breed = 'Boxer'
 ORDER BY 
     cf.file_name ASC
-LIMIT 100;</t>
-  </si>
-  <si>
-    <t>SELECT
-    DISTINCT c.case_record_id AS "Case ID",
-    st.clinical_study_designation AS "Study Code",
-    st.clinical_study_type AS "Study Type",
-    dmg.breed AS "Breed",
-    diag.disease_term AS "Diagnosis",
-    diag.stage_of_disease AS "Stage Of Disease",
-    CASE 
-    WHEN dmg.patient_age_at_enrollment = CAST(dmg.patient_age_at_enrollment AS INT) 
-    THEN CAST(CAST(dmg.patient_age_at_enrollment AS INT) AS TEXT)
-    ELSE CAST(dmg.patient_age_at_enrollment AS TEXT)
-END AS "Age", 
-    COALESCE(dmg.sex, '') AS "Sex",   
-    COALESCE(dmg.neutered_indicator, '') AS "Neutered Status",  
-    COALESCE(
-        CASE 
-            WHEN dmg.weight = CAST(dmg.weight AS INT) THEN CAST(dmg.weight AS INT)
-            ELSE dmg.weight 
-        END, 
-    '') AS "Weight (kg)",        
-    COALESCE(diag.best_response, '') AS "Response to Treatment",  
-    COALESCE(coh.cohort_description, '') AS "Cohort"  
-FROM 
-    df_case c
-JOIN 
-    df_study st ON c."study.clinical_study_designation" = st.clinical_study_designation
-JOIN 
-    df_demographic dmg ON dmg."case.case_record_id" = c.case_record_id
-JOIN 
-    df_diagnosis diag ON diag."case.case_record_id" = c.case_record_id
-JOIN 
-    df_enrollment enr ON enr."case.case_record_id" = c.case_record_id
-JOIN 
-    df_program p ON st."program.program_acronym" = p.program_acronym
-JOIN 
-    df_sample smp ON smp."case.case_record_id" = c.case_record_id
-JOIN 
-    df_publication pub ON pub."study.clinical_study_designation" = st.clinical_study_designation
-LEFT JOIN 
-    df_case_file cf ON cf."sample.sample_id" = smp.sample_id
-LEFT JOIN 
-    df_study_file sf ON sf."study.clinical_study_designation" = st.clinical_study_designation
-LEFT JOIN
-    df_cohort coh ON coh."study.clinical_study_designation" = st.clinical_study_designation
-WHERE
-    st.clinical_study_designation = 'OSA03' AND dmg.breed = 'Boxer'
-ORDER BY 
-    c.case_record_id ASC
-LIMIT 100;</t>
-  </si>
-  <si>
-    <t>SELECT DISTINCT
-    smp.sample_id AS "Sample ID",
-    c.case_record_id AS "Case ID",
-    COALESCE(dmg.breed, '') AS "Breed",
-    COALESCE(diag.disease_term, '') AS "Diagnosis",
-    COALESCE(smp.sample_site, '') AS "Sample Site",
-    COALESCE(smp.summarized_sample_type, '') AS "Sample Type",
-    COALESCE(smp.specific_sample_pathology, '') AS "Pathology/Morphology",
-    COALESCE(smp.tumor_grade, '') AS "Tumor Grade",
-    COALESCE(smp.sample_chronology, '') AS "Sample Chronology",
-    COALESCE(smp.percentage_tumor, '') AS "Percentage Tumor",
-    COALESCE(smp.necropsy_sample, '') AS "Necropsy Sample",
-    COALESCE(smp.sample_preservation, '') AS "Sample Preservation"
-FROM 
-    df_sample smp
-JOIN 
-    df_case c ON smp."case.case_record_id" = c.case_record_id
-JOIN 
-    df_publication pub ON pub."study.clinical_study_designation" = st.clinical_study_designation
-JOIN 
-    df_demographic dmg ON dmg."case.case_record_id" = c.case_record_id
-JOIN 
-    df_diagnosis diag ON diag."case.case_record_id" = c.case_record_id
-JOIN 
-    df_enrollment enr ON enr."case.case_record_id" = c.case_record_id
-JOIN 
-    df_program p ON st."program.program_acronym" = p.program_acronym
-JOIN 
-    df_study st ON c."study.clinical_study_designation" = st.clinical_study_designation
-LEFT JOIN 
-    df_case_file cf ON cf."sample.sample_id" = smp.sample_id
-LEFT JOIN 
-    df_study_file sf ON sf."study.clinical_study_designation" = st.clinical_study_designation
-WHERE 
-   st.clinical_study_designation = 'OSA03' AND dmg.breed = 'Boxer'
-ORDER BY 
-    smp.sample_id ASC
 LIMIT 100;</t>
   </si>
   <si>
@@ -284,6 +237,8 @@
 JOIN 
     df_publication pub ON pub."study.clinical_study_designation" = st.clinical_study_designation
 LEFT JOIN 
+    df_registration reg ON reg."case.case_record_id" = c.case_record_id
+LEFT JOIN 
     df_study_file sf ON sf."study.clinical_study_designation" = st.clinical_study_designation
 WHERE
     st.clinical_study_designation = 'OSA03' AND dmg.breed = 'Boxer'
@@ -314,11 +269,66 @@
 JOIN 
     df_sample smp ON smp."case.case_record_id" = c.case_record_id
 LEFT JOIN 
+    df_registration reg ON reg."case.case_record_id" = c.case_record_id
+LEFT JOIN 
     df_case_file cf ON cf."sample.sample_id" = smp.sample_id
 LEFT JOIN 
     df_study_file sf ON sf."study.clinical_study_designation" = st.clinical_study_designation
 WHERE 
     st.clinical_study_designation = 'OSA03' AND dmg.breed = 'Boxer';</t>
+  </si>
+  <si>
+    <t>SELECT
+    DISTINCT c.case_record_id AS "Case ID",
+    st.clinical_study_designation AS "Study Code",
+    st.clinical_study_type AS "Study Type",
+    dmg.breed AS "Breed",
+    diag.disease_term AS "Diagnosis",
+    diag.stage_of_disease AS "Stage Of Disease",
+    CASE 
+    WHEN dmg.patient_age_at_enrollment = CAST(dmg.patient_age_at_enrollment AS INT) 
+    THEN CAST(CAST(dmg.patient_age_at_enrollment AS INT) AS TEXT)
+    ELSE CAST(dmg.patient_age_at_enrollment AS TEXT)
+END AS "Age", 
+    COALESCE(TRIM(dmg.sex), '') AS "Sex",   
+    COALESCE(dmg.neutered_indicator, '') AS "Neutered Status",  
+    COALESCE(
+    CASE 
+        WHEN dmg.weight = CAST(dmg.weight AS INT) THEN TRIM(CAST(dmg.weight AS TEXT), '.0')
+        ELSE CAST(ROUND(dmg.weight, 1) AS TEXT)
+    END, 
+'') AS "Weight (kg)",        
+    COALESCE(diag.best_response, '') AS "Response to Treatment",  
+    COALESCE(coh.cohort_description, '') AS "Cohort"  
+FROM 
+    df_case c
+JOIN 
+    df_study st ON c."study.clinical_study_designation" = st.clinical_study_designation
+JOIN 
+    df_demographic dmg ON dmg."case.case_record_id" = c.case_record_id
+JOIN 
+    df_diagnosis diag ON diag."case.case_record_id" = c.case_record_id
+JOIN 
+    df_enrollment enr ON enr."case.case_record_id" = c.case_record_id
+JOIN 
+    df_program p ON st."program.program_acronym" = p.program_acronym
+JOIN 
+    df_sample smp ON smp."case.case_record_id" = c.case_record_id
+JOIN 
+    df_publication pub ON pub."study.clinical_study_designation" = st.clinical_study_designation
+LEFT JOIN 
+    df_case_file cf ON cf."sample.sample_id" = smp.sample_id
+LEFT JOIN 
+    df_registration reg ON reg."case.case_record_id" = c.case_record_id
+LEFT JOIN 
+    df_study_file sf ON sf."study.clinical_study_designation" = st.clinical_study_designation
+LEFT JOIN
+    df_cohort coh ON coh."study.clinical_study_designation" = st.clinical_study_designation
+WHERE
+    st.clinical_study_designation = 'OSA03' AND dmg.breed = 'Boxer'
+ORDER BY 
+    c.case_record_id ASC
+LIMIT 100;</t>
   </si>
 </sst>
 </file>
@@ -721,7 +731,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -754,10 +764,10 @@
         <v>6</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2" s="4" t="s">
         <v>15</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>14</v>
       </c>
       <c r="D2" t="s">
         <v>10</v>
@@ -771,7 +781,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C3" s="2"/>
     </row>
@@ -780,7 +790,7 @@
         <v>8</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C4" s="2"/>
     </row>
@@ -789,7 +799,7 @@
         <v>7</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C5" s="1"/>
     </row>

</xml_diff>